<commit_message>
Table data for paper 2
after second round of revisions
</commit_message>
<xml_diff>
--- a/Data_and_Analysis_Scripts/table_data.xlsx
+++ b/Data_and_Analysis_Scripts/table_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwnetid-my.sharepoint.com/personal/apolet_uw_edu/Documents/Documents/Winter 2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{73BB393E-6A4D-4847-A7A5-D246602DEC14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="534" documentId="8_{73BB393E-6A4D-4847-A7A5-D246602DEC14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02663E5D-3DF6-45F7-9D8A-679ECFA7200D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FBC4E8BD-05EE-41DD-8D91-9CC51D6AD49B}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="62">
   <si>
     <t>Model</t>
   </si>
@@ -77,13 +78,7 @@
     <t>Standard Deviation</t>
   </si>
   <si>
-    <t>EffCS Difference</t>
-  </si>
-  <si>
     <t>dT/dt Difference</t>
-  </si>
-  <si>
-    <t>ERF Difference</t>
   </si>
   <si>
     <t>λ Difference</t>
@@ -178,22 +173,6 @@
         <family val="1"/>
       </rPr>
       <t xml:space="preserve">2xCO2 </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>ERF</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">4xCO2 </t>
     </r>
   </si>
   <si>
@@ -472,33 +451,9 @@
     <t>Unit</t>
   </si>
   <si>
-    <t>Effective Climate Sensitivity</t>
-  </si>
-  <si>
-    <t>Slope of Slow Period Temperature Change</t>
-  </si>
-  <si>
-    <t>Effective Radiative Forcing</t>
-  </si>
-  <si>
-    <t>Radiative Feedback Parameter</t>
-  </si>
-  <si>
-    <t>Effective Heat Capacity</t>
-  </si>
-  <si>
-    <t>EBM Relative Importance</t>
-  </si>
-  <si>
-    <t>Change in AMOC Strength</t>
-  </si>
-  <si>
     <t>Ratio of AMOC Change</t>
   </si>
   <si>
-    <t>Northern Hemisphere Depth of Heat Storage</t>
-  </si>
-  <si>
     <t>Northern Hemisphere Temperature Regressed Against Global Mean</t>
   </si>
   <si>
@@ -512,6 +467,87 @@
   </si>
   <si>
     <t>[K/K]</t>
+  </si>
+  <si>
+    <t>EffCS Difference (between 2x and 4x)</t>
+  </si>
+  <si>
+    <r>
+      <t>ERF</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">4xCO2, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Smith et al. (2020)</t>
+    </r>
+  </si>
+  <si>
+    <t>ERF Ratio</t>
+  </si>
+  <si>
+    <t>Radiative Feedback Parameter (Table 1d)</t>
+  </si>
+  <si>
+    <t>Effective Radiative Forcing and Scaling Ratio (Table 1c)</t>
+  </si>
+  <si>
+    <t>Slope of Slow Period Temperature Change (Table 1a)</t>
+  </si>
+  <si>
+    <t>Effective Climate Sensitivity, ERF Scaling (Table 1b)</t>
+  </si>
+  <si>
+    <t>Effective Heat Capacity, Final 20 Year Average (Table 2a)</t>
+  </si>
+  <si>
+    <t>EBM Relative Importance (Table 2b)</t>
+  </si>
+  <si>
+    <t>Change in AMOC Strength (Table 2c)</t>
+  </si>
+  <si>
+    <t>Northern Hemisphere Depth of Heat Storage (Table 2d)</t>
+  </si>
+  <si>
+    <t>GISS-E2-2-G</t>
+  </si>
+  <si>
+    <t>HadGEM3-GC31-LL</t>
+  </si>
+  <si>
+    <r>
+      <t>ERF</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>4xCO2</t>
+    </r>
+  </si>
+  <si>
+    <t>Percent Difference (From Smith et al.)</t>
   </si>
 </sst>
 </file>
@@ -522,7 +558,7 @@
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -594,6 +630,35 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -609,7 +674,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -632,11 +697,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -678,22 +780,75 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -710,6 +865,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1009,183 +1168,196 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEE8EAC5-F3EB-4440-AA06-40799DC25633}">
-  <dimension ref="A1:AC13"/>
+  <dimension ref="A1:AE30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="T1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.6640625" style="13" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="12.77734375" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.21875" style="13" customWidth="1"/>
-    <col min="8" max="9" width="13.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13" style="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="13.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="17" width="13.88671875" style="13" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14" style="13" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.88671875" style="13" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.5546875" style="13" customWidth="1"/>
-    <col min="21" max="21" width="14" style="13" customWidth="1"/>
-    <col min="22" max="22" width="21.109375" style="13" customWidth="1"/>
-    <col min="23" max="23" width="12.109375" style="13" customWidth="1"/>
-    <col min="24" max="24" width="13.77734375" style="13" customWidth="1"/>
-    <col min="25" max="25" width="14.88671875" style="13" customWidth="1"/>
-    <col min="26" max="26" width="25.44140625" style="13" customWidth="1"/>
-    <col min="27" max="27" width="26.77734375" style="13" customWidth="1"/>
-    <col min="28" max="28" width="25.109375" style="13" customWidth="1"/>
-    <col min="29" max="29" width="27" style="13" customWidth="1"/>
-    <col min="30" max="16384" width="8.88671875" style="13"/>
+    <col min="2" max="2" width="12.33203125" style="13" customWidth="1"/>
+    <col min="3" max="3" width="12.77734375" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" style="13" customWidth="1"/>
+    <col min="5" max="6" width="13.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.77734375" style="13" customWidth="1"/>
+    <col min="8" max="8" width="13" style="13" customWidth="1"/>
+    <col min="9" max="10" width="13.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.88671875" style="13" customWidth="1"/>
+    <col min="12" max="14" width="13.88671875" style="13" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14" style="13" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.88671875" style="13" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.5546875" style="13" customWidth="1"/>
+    <col min="18" max="18" width="15.33203125" style="13" customWidth="1"/>
+    <col min="19" max="19" width="21.109375" style="13" customWidth="1"/>
+    <col min="20" max="20" width="12.109375" style="13" customWidth="1"/>
+    <col min="21" max="21" width="13.77734375" style="13" customWidth="1"/>
+    <col min="22" max="22" width="14.88671875" style="13" customWidth="1"/>
+    <col min="23" max="23" width="15.44140625" style="13" customWidth="1"/>
+    <col min="24" max="24" width="21.77734375" style="13" customWidth="1"/>
+    <col min="25" max="25" width="15.88671875" style="13" customWidth="1"/>
+    <col min="26" max="26" width="19.5546875" style="13" customWidth="1"/>
+    <col min="27" max="27" width="13.33203125" style="13" customWidth="1"/>
+    <col min="28" max="28" width="26.6640625" style="13" customWidth="1"/>
+    <col min="29" max="29" width="28.109375" style="13" customWidth="1"/>
+    <col min="30" max="30" width="27.33203125" style="13" customWidth="1"/>
+    <col min="31" max="31" width="27.5546875" style="13" customWidth="1"/>
+    <col min="32" max="16384" width="8.88671875" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14"/>
-      <c r="B1" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15" t="s">
+      <c r="B1" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="36"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="X1" s="15"/>
-      <c r="Y1" s="15"/>
-      <c r="Z1" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="AA1" s="15"/>
-      <c r="AB1" s="15" t="s">
+      <c r="N1" s="36"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="AC1" s="15"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="37"/>
+      <c r="S1" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="T1" s="36"/>
+      <c r="U1" s="37"/>
+      <c r="V1" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="W1" s="36"/>
+      <c r="X1" s="37"/>
+      <c r="Y1" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z1" s="36"/>
+      <c r="AA1" s="37"/>
+      <c r="AB1" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC1" s="37"/>
+      <c r="AD1" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE1" s="37"/>
     </row>
-    <row r="2" spans="1:29" ht="15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:31" ht="54" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="I2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J2" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L2" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="N2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="U2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="O2" s="2" t="s">
+      <c r="V2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="P2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="R2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="T2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="AB2" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC2" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD2" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE2" s="15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z2" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="AA2" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB2" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="AC2" s="16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>1</v>
@@ -1197,82 +1369,88 @@
         <v>2</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="J3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="17" t="s">
         <v>2</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
+      </c>
+      <c r="L3" s="19" t="s">
+        <v>2</v>
       </c>
       <c r="M3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="N3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="P3" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="S3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="T3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="Z3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="V3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="W3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="X3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="Z3" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="AA3" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB3" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="AC3" s="17" t="s">
-        <v>57</v>
+      <c r="AA3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="AB3" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC3" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD3" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE3" s="14" t="s">
+        <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1280,290 +1458,311 @@
         <v>4.67</v>
       </c>
       <c r="C4" s="3">
-        <v>5.39</v>
+        <v>5.35</v>
       </c>
       <c r="D4" s="7">
         <f>(C4-B4)/C4</f>
-        <v>0.13358070500927641</v>
+        <v>0.1271028037383177</v>
       </c>
       <c r="E4" s="3">
-        <v>5.82</v>
+        <v>6.51</v>
       </c>
       <c r="F4" s="3">
-        <v>7.21</v>
+        <v>7.84</v>
       </c>
       <c r="G4" s="7">
         <f>(F4-E4)/F4</f>
-        <v>0.19278779472954227</v>
+        <v>0.16964285714285715</v>
       </c>
       <c r="H4" s="3">
-        <v>3.78</v>
+        <v>3.53</v>
       </c>
       <c r="I4" s="3">
-        <v>3.62</v>
-      </c>
-      <c r="J4" s="7">
-        <f t="shared" ref="J4:J11" si="0">(I4-H4)/I4</f>
-        <v>-4.4198895027624224E-2</v>
-      </c>
-      <c r="K4" s="3">
+        <v>7.46</v>
+      </c>
+      <c r="J4" s="31">
+        <f>H4/I4</f>
+        <v>0.47319034852546915</v>
+      </c>
+      <c r="K4" s="25">
+        <v>7.61</v>
+      </c>
+      <c r="L4" s="29">
+        <f>(I4-K4)/I4</f>
+        <v>-2.0107238605898171E-2</v>
+      </c>
+      <c r="M4" s="3">
         <v>-0.76</v>
       </c>
-      <c r="L4" s="3">
+      <c r="N4" s="3">
         <v>-0.66</v>
       </c>
-      <c r="M4" s="7">
-        <f>(L4-K4)/L4</f>
+      <c r="O4" s="7">
+        <f>(N4-M4)/N4</f>
         <v>-0.15151515151515146</v>
       </c>
-      <c r="N4" s="3">
+      <c r="P4" s="3">
         <v>1.54</v>
       </c>
-      <c r="O4" s="3">
+      <c r="Q4" s="3">
         <v>1.55</v>
       </c>
-      <c r="P4" s="3">
-        <f>N4-O4</f>
+      <c r="R4" s="3">
+        <f>P4-Q4</f>
         <v>-1.0000000000000009E-2</v>
       </c>
-      <c r="Q4" s="3">
-        <v>101.77</v>
-      </c>
-      <c r="R4" s="3">
-        <v>-2.8</v>
-      </c>
       <c r="S4" s="3">
-        <f>100-Q4-R4</f>
-        <v>1.0300000000000038</v>
-      </c>
-      <c r="T4" s="3">
+        <v>101.89</v>
+      </c>
+      <c r="T4" s="27">
+        <v>-2.96</v>
+      </c>
+      <c r="U4" s="3">
+        <f>100-S4-T4</f>
+        <v>1.0699999999999994</v>
+      </c>
+      <c r="V4" s="3">
         <v>-3.03</v>
       </c>
-      <c r="U4" s="3">
+      <c r="W4" s="3">
         <v>-7.98</v>
       </c>
-      <c r="V4" s="8">
-        <f>T4/U4</f>
+      <c r="X4" s="8">
+        <f>V4/W4</f>
         <v>0.3796992481203007</v>
       </c>
-      <c r="W4" s="3">
+      <c r="Y4" s="3">
         <v>587</v>
       </c>
-      <c r="X4" s="3">
+      <c r="Z4" s="3">
         <v>505</v>
       </c>
-      <c r="Y4" s="3">
-        <f>W4-X4</f>
+      <c r="AA4" s="3">
+        <f>Y4-Z4</f>
         <v>82</v>
       </c>
-      <c r="Z4" s="18">
+      <c r="AB4" s="21">
         <v>1.21</v>
       </c>
-      <c r="AA4" s="18">
+      <c r="AC4" s="21">
         <v>1.04</v>
       </c>
-      <c r="AB4" s="18">
+      <c r="AD4" s="21">
         <v>0.79</v>
       </c>
-      <c r="AC4" s="18">
+      <c r="AE4" s="21">
         <v>0.96</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2">
         <v>3.37</v>
       </c>
-      <c r="C5" s="2">
-        <v>4.99</v>
+      <c r="C5" s="30">
+        <v>6.4</v>
       </c>
       <c r="D5" s="9">
-        <f t="shared" ref="D5:D11" si="1">(C5-B5)/C5</f>
-        <v>0.32464929859719438</v>
+        <f t="shared" ref="D5:D13" si="0">(C5-B5)/C5</f>
+        <v>0.47343750000000001</v>
       </c>
       <c r="E5" s="2">
-        <v>3.9</v>
+        <v>4.17</v>
       </c>
       <c r="F5" s="2">
-        <v>9.27</v>
+        <v>12.3</v>
       </c>
       <c r="G5" s="9">
-        <f t="shared" ref="G5:G11" si="2">(F5-E5)/F5</f>
-        <v>0.57928802588996753</v>
+        <f t="shared" ref="G5:G13" si="1">(F5-E5)/F5</f>
+        <v>0.66097560975609759</v>
       </c>
       <c r="H5" s="2">
-        <v>4.55</v>
+        <v>4.0599999999999996</v>
       </c>
       <c r="I5" s="2">
-        <v>4.08</v>
-      </c>
-      <c r="J5" s="9">
-        <f t="shared" si="0"/>
-        <v>-0.11519607843137249</v>
-      </c>
-      <c r="K5" s="2">
+        <v>6.65</v>
+      </c>
+      <c r="J5" s="32">
+        <f t="shared" ref="J5:J13" si="2">H5/I5</f>
+        <v>0.61052631578947358</v>
+      </c>
+      <c r="K5" s="26">
+        <v>8.91</v>
+      </c>
+      <c r="L5" s="29">
+        <f>(I5-K5)/I5</f>
+        <v>-0.33984962406015035</v>
+      </c>
+      <c r="M5" s="2">
         <v>-1.21</v>
       </c>
-      <c r="L5" s="2">
+      <c r="N5" s="2">
         <v>-0.63</v>
       </c>
-      <c r="M5" s="9">
-        <f t="shared" ref="M5:M11" si="3">(L5-K5)/L5</f>
+      <c r="O5" s="9">
+        <f t="shared" ref="O5:O13" si="3">(N5-M5)/N5</f>
         <v>-0.92063492063492058</v>
       </c>
-      <c r="N5" s="2">
+      <c r="P5" s="2">
         <v>2.61</v>
       </c>
-      <c r="O5" s="2">
+      <c r="Q5" s="2">
         <v>1.79</v>
       </c>
-      <c r="P5" s="2">
-        <f t="shared" ref="P5:P11" si="4">N5-O5</f>
+      <c r="R5" s="2">
+        <f t="shared" ref="R5:R13" si="4">P5-Q5</f>
         <v>0.81999999999999984</v>
       </c>
-      <c r="Q5" s="2">
-        <v>62.49</v>
-      </c>
-      <c r="R5" s="2">
-        <v>64.180000000000007</v>
-      </c>
       <c r="S5" s="2">
-        <f t="shared" ref="S5:S11" si="5">100-Q5-R5</f>
-        <v>-26.670000000000009</v>
+        <v>80.760000000000005</v>
       </c>
       <c r="T5" s="2">
+        <v>42.24</v>
+      </c>
+      <c r="U5" s="30">
+        <f t="shared" ref="U5:U13" si="5">100-S5-T5</f>
+        <v>-23.000000000000007</v>
+      </c>
+      <c r="V5" s="2">
         <v>-15.24</v>
       </c>
-      <c r="U5" s="2">
+      <c r="W5" s="2">
         <v>-20.87</v>
       </c>
-      <c r="V5" s="10">
-        <f t="shared" ref="V5:V11" si="6">T5/U5</f>
+      <c r="X5" s="10">
+        <f t="shared" ref="X5:X13" si="6">V5/W5</f>
         <v>0.73023478677527554</v>
       </c>
-      <c r="W5" s="2">
+      <c r="Y5" s="2">
         <v>697</v>
       </c>
-      <c r="X5" s="2">
+      <c r="Z5" s="2">
         <v>574</v>
       </c>
-      <c r="Y5" s="2">
-        <f t="shared" ref="Y5:Y11" si="7">W5-X5</f>
+      <c r="AA5" s="2">
+        <f t="shared" ref="AA5:AA13" si="7">Y5-Z5</f>
         <v>123</v>
       </c>
-      <c r="Z5" s="19">
+      <c r="AB5" s="22">
         <v>0.4</v>
       </c>
-      <c r="AA5" s="19">
+      <c r="AC5" s="22">
         <v>0.82</v>
       </c>
-      <c r="AB5" s="20">
+      <c r="AD5" s="23">
         <v>1.6</v>
       </c>
-      <c r="AC5" s="19">
+      <c r="AE5" s="22">
         <v>1.18</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="27">
         <v>4.2</v>
       </c>
       <c r="C6" s="3">
-        <v>4.63</v>
+        <v>4.46</v>
       </c>
       <c r="D6" s="7">
+        <f t="shared" si="0"/>
+        <v>5.8295964125560491E-2</v>
+      </c>
+      <c r="E6" s="3">
+        <v>7.78</v>
+      </c>
+      <c r="F6" s="3">
+        <v>5.15</v>
+      </c>
+      <c r="G6" s="7">
         <f t="shared" si="1"/>
-        <v>9.2872570194384385E-2</v>
-      </c>
-      <c r="E6" s="3">
-        <v>7.74</v>
-      </c>
-      <c r="F6" s="3">
-        <v>4.79</v>
-      </c>
-      <c r="G6" s="7">
+        <v>-0.51067961165048537</v>
+      </c>
+      <c r="H6" s="3">
+        <v>3.27</v>
+      </c>
+      <c r="I6" s="3">
+        <v>7.11</v>
+      </c>
+      <c r="J6" s="31">
         <f t="shared" si="2"/>
-        <v>-0.61586638830897711</v>
-      </c>
-      <c r="H6" s="3">
-        <v>3.76</v>
-      </c>
-      <c r="I6" s="3">
-        <v>3.65</v>
-      </c>
-      <c r="J6" s="7">
-        <f t="shared" si="0"/>
-        <v>-3.0136986301369829E-2</v>
-      </c>
-      <c r="K6" s="3">
+        <v>0.45991561181434598</v>
+      </c>
+      <c r="K6" s="25">
+        <v>8</v>
+      </c>
+      <c r="L6" s="29">
+        <f>(I6-K6)/I6</f>
+        <v>-0.12517580872011247</v>
+      </c>
+      <c r="M6" s="3">
         <v>-0.78</v>
       </c>
-      <c r="L6" s="3">
+      <c r="N6" s="3">
         <v>-0.73</v>
       </c>
-      <c r="M6" s="7">
+      <c r="O6" s="7">
         <f t="shared" si="3"/>
         <v>-6.8493150684931572E-2</v>
       </c>
-      <c r="N6" s="3">
+      <c r="P6" s="3">
         <v>1.93</v>
       </c>
-      <c r="O6" s="3">
+      <c r="Q6" s="3">
         <v>1.89</v>
       </c>
-      <c r="P6" s="3">
+      <c r="R6" s="3">
         <f t="shared" si="4"/>
         <v>4.0000000000000036E-2</v>
       </c>
-      <c r="Q6" s="3">
-        <v>152.33000000000001</v>
-      </c>
-      <c r="R6" s="3">
-        <v>-54.86</v>
-      </c>
       <c r="S6" s="3">
+        <v>297.69</v>
+      </c>
+      <c r="T6" s="3">
+        <v>-199.97</v>
+      </c>
+      <c r="U6" s="3">
         <f t="shared" si="5"/>
-        <v>2.5299999999999869</v>
-      </c>
-      <c r="T6" s="3">
+        <v>2.2800000000000011</v>
+      </c>
+      <c r="V6" s="3">
         <v>-10.220000000000001</v>
       </c>
-      <c r="U6" s="3">
+      <c r="W6" s="3">
         <v>-16.29</v>
       </c>
-      <c r="V6" s="8">
+      <c r="X6" s="8">
         <f t="shared" si="6"/>
         <v>0.62737875997544512</v>
       </c>
-      <c r="W6" s="3">
+      <c r="Y6" s="3">
         <v>655</v>
       </c>
-      <c r="X6" s="3">
+      <c r="Z6" s="3">
         <v>603</v>
       </c>
-      <c r="Y6" s="3">
+      <c r="AA6" s="3">
         <f t="shared" si="7"/>
         <v>52</v>
       </c>
-      <c r="Z6" s="18">
+      <c r="AB6" s="21">
         <v>0.9</v>
       </c>
-      <c r="AA6" s="18">
+      <c r="AC6" s="21">
         <v>0.88</v>
       </c>
-      <c r="AB6" s="21">
+      <c r="AD6" s="24">
         <v>1.1000000000000001</v>
       </c>
-      <c r="AC6" s="18">
+      <c r="AE6" s="21">
         <v>1.1200000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
@@ -1571,712 +1770,960 @@
         <v>2.63</v>
       </c>
       <c r="C7" s="5">
-        <v>2.57</v>
-      </c>
-      <c r="D7" s="11">
+        <v>2.62</v>
+      </c>
+      <c r="D7" s="7">
+        <f t="shared" si="0"/>
+        <v>-3.8167938931296893E-3</v>
+      </c>
+      <c r="E7" s="5">
+        <v>4.43</v>
+      </c>
+      <c r="F7" s="5">
+        <v>2.54</v>
+      </c>
+      <c r="G7" s="11">
         <f t="shared" si="1"/>
-        <v>-2.3346303501945546E-2</v>
-      </c>
-      <c r="E7" s="5">
-        <v>4.42</v>
-      </c>
-      <c r="F7" s="5">
-        <v>2.61</v>
-      </c>
-      <c r="G7" s="11">
+        <v>-0.74409448818897628</v>
+      </c>
+      <c r="H7" s="5">
+        <v>3.78</v>
+      </c>
+      <c r="I7" s="5">
+        <v>7.81</v>
+      </c>
+      <c r="J7" s="31">
         <f t="shared" si="2"/>
-        <v>-0.69348659003831425</v>
-      </c>
-      <c r="H7" s="5">
-        <v>4.12</v>
-      </c>
-      <c r="I7" s="5">
-        <v>3.73</v>
-      </c>
-      <c r="J7" s="11">
-        <f t="shared" si="0"/>
-        <v>-0.10455764075067027</v>
-      </c>
-      <c r="K7" s="5">
+        <v>0.48399487836107552</v>
+      </c>
+      <c r="K7" s="25">
+        <v>7.35</v>
+      </c>
+      <c r="L7" s="29">
+        <f>(I7-K7)/I7</f>
+        <v>5.8898847631241993E-2</v>
+      </c>
+      <c r="M7" s="5">
         <v>-1.43</v>
       </c>
-      <c r="L7" s="5">
+      <c r="N7" s="5">
         <v>-1.44</v>
       </c>
-      <c r="M7" s="11">
+      <c r="O7" s="11">
         <f t="shared" si="3"/>
         <v>6.944444444444451E-3</v>
       </c>
-      <c r="N7" s="5">
+      <c r="P7" s="5">
         <v>2.2599999999999998</v>
       </c>
-      <c r="O7" s="5">
+      <c r="Q7" s="5">
         <v>2.4900000000000002</v>
       </c>
-      <c r="P7" s="5">
+      <c r="R7" s="5">
         <f t="shared" si="4"/>
         <v>-0.23000000000000043</v>
       </c>
-      <c r="Q7" s="5">
-        <v>35.130000000000003</v>
-      </c>
-      <c r="R7" s="5">
-        <v>63.13</v>
-      </c>
       <c r="S7" s="5">
+        <v>11.02</v>
+      </c>
+      <c r="T7" s="34">
+        <v>87.98</v>
+      </c>
+      <c r="U7" s="6">
         <f t="shared" si="5"/>
-        <v>1.740000000000002</v>
-      </c>
-      <c r="T7" s="5">
+        <v>1</v>
+      </c>
+      <c r="V7" s="5">
         <v>0.87</v>
       </c>
-      <c r="U7" s="5">
+      <c r="W7" s="5">
         <v>-19.260000000000002</v>
       </c>
-      <c r="V7" s="11">
+      <c r="X7" s="11">
         <f t="shared" si="6"/>
         <v>-4.5171339563862926E-2</v>
       </c>
-      <c r="W7" s="5">
+      <c r="Y7" s="5">
         <v>958</v>
       </c>
-      <c r="X7" s="5">
+      <c r="Z7" s="5">
         <v>839</v>
       </c>
-      <c r="Y7" s="5">
+      <c r="AA7" s="5">
         <f t="shared" si="7"/>
         <v>119</v>
       </c>
-      <c r="Z7" s="18">
+      <c r="AB7" s="21">
         <v>1.22</v>
       </c>
-      <c r="AA7" s="18">
+      <c r="AC7" s="21">
         <v>0.68</v>
       </c>
-      <c r="AB7" s="18">
+      <c r="AD7" s="21">
         <v>0.78</v>
       </c>
-      <c r="AC7" s="18">
+      <c r="AE7" s="21">
         <v>1.32</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="5">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="C8" s="5">
+        <v>2.36</v>
+      </c>
+      <c r="D8" s="7">
+        <f t="shared" si="0"/>
+        <v>-5.5084745762712009E-2</v>
+      </c>
+      <c r="E8" s="5">
+        <v>2.71</v>
+      </c>
+      <c r="F8" s="33">
+        <v>0.44</v>
+      </c>
+      <c r="G8" s="11">
+        <f t="shared" si="1"/>
+        <v>-5.1590909090909092</v>
+      </c>
+      <c r="H8" s="5">
+        <v>3.74</v>
+      </c>
+      <c r="I8" s="5">
+        <v>7.59</v>
+      </c>
+      <c r="J8" s="31">
+        <f t="shared" si="2"/>
+        <v>0.49275362318840582</v>
+      </c>
+      <c r="K8" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="M8" s="6">
+        <v>-1.5</v>
+      </c>
+      <c r="N8" s="5">
+        <v>-1.59</v>
+      </c>
+      <c r="O8" s="11">
+        <f t="shared" si="3"/>
+        <v>5.660377358490571E-2</v>
+      </c>
+      <c r="P8" s="5">
+        <v>1.43</v>
+      </c>
+      <c r="Q8" s="6">
+        <v>2.1</v>
+      </c>
+      <c r="R8" s="5">
+        <f t="shared" si="4"/>
+        <v>-0.67000000000000015</v>
+      </c>
+      <c r="S8" s="5">
+        <v>30.07</v>
+      </c>
+      <c r="T8" s="34">
+        <v>63.69</v>
+      </c>
+      <c r="U8" s="6">
+        <f t="shared" si="5"/>
+        <v>6.2400000000000091</v>
+      </c>
+      <c r="V8" s="5"/>
+      <c r="W8" s="5"/>
+      <c r="X8" s="11"/>
+      <c r="Y8" s="5"/>
+      <c r="Z8" s="5"/>
+      <c r="AA8" s="5"/>
+      <c r="AB8" s="21"/>
+      <c r="AC8" s="21"/>
+      <c r="AD8" s="21"/>
+      <c r="AE8" s="21"/>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B9" s="3">
         <v>2.96</v>
       </c>
-      <c r="C8" s="3">
-        <v>2.95</v>
-      </c>
-      <c r="D8" s="7">
+      <c r="C9" s="27">
+        <v>3.2</v>
+      </c>
+      <c r="D9" s="7">
+        <f t="shared" si="0"/>
+        <v>7.5000000000000067E-2</v>
+      </c>
+      <c r="E9" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="F9" s="3">
+        <v>4.18</v>
+      </c>
+      <c r="G9" s="7">
         <f t="shared" si="1"/>
-        <v>-3.3898305084745037E-3</v>
-      </c>
-      <c r="E8" s="3">
-        <v>3.54</v>
-      </c>
-      <c r="F8" s="3">
-        <v>3.6</v>
-      </c>
-      <c r="G8" s="7">
+        <v>6.6985645933014315E-2</v>
+      </c>
+      <c r="H9" s="3">
+        <v>3.76</v>
+      </c>
+      <c r="I9" s="3">
+        <v>7.28</v>
+      </c>
+      <c r="J9" s="31">
         <f t="shared" si="2"/>
-        <v>1.666666666666668E-2</v>
-      </c>
-      <c r="H8" s="3">
-        <v>3.97</v>
-      </c>
-      <c r="I8" s="3">
-        <v>3.6</v>
-      </c>
-      <c r="J8" s="7">
-        <f t="shared" si="0"/>
-        <v>-0.1027777777777778</v>
-      </c>
-      <c r="K8" s="3">
+        <v>0.51648351648351642</v>
+      </c>
+      <c r="K9" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="M9" s="3">
         <v>-1.27</v>
       </c>
-      <c r="L8" s="3">
+      <c r="N9" s="3">
         <v>-1.17</v>
       </c>
-      <c r="M8" s="7">
+      <c r="O9" s="7">
         <f t="shared" si="3"/>
         <v>-8.5470085470085555E-2</v>
       </c>
-      <c r="N8" s="3">
+      <c r="P9" s="3">
         <v>1.91</v>
       </c>
-      <c r="O8" s="3">
+      <c r="Q9" s="3">
         <v>1.88</v>
       </c>
-      <c r="P8" s="3">
+      <c r="R9" s="3">
         <f t="shared" si="4"/>
         <v>3.0000000000000027E-2</v>
       </c>
-      <c r="Q8" s="3">
-        <v>122.97</v>
-      </c>
-      <c r="R8" s="3">
-        <v>-26.63</v>
-      </c>
-      <c r="S8" s="3">
+      <c r="S9" s="3">
+        <v>94.48</v>
+      </c>
+      <c r="T9" s="3">
+        <v>6.93</v>
+      </c>
+      <c r="U9" s="3">
         <f t="shared" si="5"/>
-        <v>3.66</v>
-      </c>
-      <c r="T8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="U8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="V8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="W8" s="3">
+        <v>-1.4100000000000037</v>
+      </c>
+      <c r="V9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="W9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="X9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y9" s="3">
         <v>683</v>
       </c>
-      <c r="X8" s="3">
+      <c r="Z9" s="3">
         <v>659</v>
       </c>
-      <c r="Y8" s="3">
+      <c r="AA9" s="3">
         <f t="shared" si="7"/>
         <v>24</v>
       </c>
-      <c r="Z8" s="18">
+      <c r="AB9" s="21">
         <v>0.97</v>
       </c>
-      <c r="AA8" s="18">
+      <c r="AC9" s="21">
         <v>0.93</v>
       </c>
-      <c r="AB8" s="18">
+      <c r="AD9" s="21">
         <v>1.03</v>
       </c>
-      <c r="AC8" s="18">
+      <c r="AE9" s="21">
         <v>1.07</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="3">
+        <v>4.88</v>
+      </c>
+      <c r="C10" s="27">
+        <v>5.36</v>
+      </c>
+      <c r="D10" s="7">
+        <f t="shared" si="0"/>
+        <v>8.9552238805970227E-2</v>
+      </c>
+      <c r="E10" s="3">
+        <v>8.7899999999999991</v>
+      </c>
+      <c r="F10" s="3">
+        <v>8.58</v>
+      </c>
+      <c r="G10" s="7">
+        <f t="shared" si="1"/>
+        <v>-2.4475524475524368E-2</v>
+      </c>
+      <c r="H10" s="3">
+        <v>3.34</v>
+      </c>
+      <c r="I10" s="3">
+        <v>6.89</v>
+      </c>
+      <c r="J10" s="31">
+        <f t="shared" si="2"/>
+        <v>0.48476052249637158</v>
+      </c>
+      <c r="K10" s="27">
+        <v>8.09</v>
+      </c>
+      <c r="L10" s="29">
+        <f>(I10-K10)/I10</f>
+        <v>-0.17416545718432513</v>
+      </c>
+      <c r="M10" s="3">
+        <v>-0.68</v>
+      </c>
+      <c r="N10" s="3">
+        <v>-0.62</v>
+      </c>
+      <c r="O10" s="7">
+        <f t="shared" si="3"/>
+        <v>-9.6774193548387177E-2</v>
+      </c>
+      <c r="P10" s="3">
+        <v>1.74</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>1.57</v>
+      </c>
+      <c r="R10" s="3">
+        <f t="shared" si="4"/>
+        <v>0.16999999999999993</v>
+      </c>
+      <c r="S10" s="3">
+        <v>65.599999999999994</v>
+      </c>
+      <c r="T10" s="3">
+        <v>39.15</v>
+      </c>
+      <c r="U10" s="3">
+        <f t="shared" si="5"/>
+        <v>-4.7499999999999929</v>
+      </c>
+      <c r="V10" s="3"/>
+      <c r="W10" s="3"/>
+      <c r="X10" s="3"/>
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="3"/>
+      <c r="AA10" s="3"/>
+      <c r="AB10" s="21"/>
+      <c r="AC10" s="21"/>
+      <c r="AD10" s="21"/>
+      <c r="AE10" s="21"/>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B11" s="3">
         <v>3.97</v>
       </c>
-      <c r="C9" s="3">
-        <v>4.37</v>
-      </c>
-      <c r="D9" s="7">
+      <c r="C11" s="27">
+        <v>4.8</v>
+      </c>
+      <c r="D11" s="7">
+        <f t="shared" si="0"/>
+        <v>0.17291666666666661</v>
+      </c>
+      <c r="E11" s="3">
+        <v>6.02</v>
+      </c>
+      <c r="F11" s="3">
+        <v>6.72</v>
+      </c>
+      <c r="G11" s="7">
         <f t="shared" si="1"/>
-        <v>9.1533180778032019E-2</v>
-      </c>
-      <c r="E9" s="3">
-        <v>5.72</v>
-      </c>
-      <c r="F9" s="3">
-        <v>5.57</v>
-      </c>
-      <c r="G9" s="7">
+        <v>0.1041666666666667</v>
+      </c>
+      <c r="H11" s="3">
+        <v>3.69</v>
+      </c>
+      <c r="I11" s="3">
+        <v>7.06</v>
+      </c>
+      <c r="J11" s="31">
         <f t="shared" si="2"/>
-        <v>-2.6929982046678538E-2</v>
-      </c>
-      <c r="H9" s="3">
-        <v>4.09</v>
-      </c>
-      <c r="I9" s="3">
-        <v>3.8</v>
-      </c>
-      <c r="J9" s="7">
-        <f t="shared" si="0"/>
-        <v>-7.6315789473684226E-2</v>
-      </c>
-      <c r="K9" s="3">
+        <v>0.52266288951841366</v>
+      </c>
+      <c r="K11" s="25">
+        <v>8</v>
+      </c>
+      <c r="L11" s="29">
+        <f>(I11-K11)/I11</f>
+        <v>-0.13314447592067996</v>
+      </c>
+      <c r="M11" s="3">
         <v>-0.93</v>
       </c>
-      <c r="L9" s="3">
+      <c r="N11" s="3">
         <v>-0.77</v>
       </c>
-      <c r="M9" s="7">
+      <c r="O11" s="7">
         <f t="shared" si="3"/>
         <v>-0.20779220779220783</v>
       </c>
-      <c r="N9" s="3">
+      <c r="P11" s="3">
         <v>1.38</v>
       </c>
-      <c r="O9" s="3">
+      <c r="Q11" s="3">
         <v>1.33</v>
       </c>
-      <c r="P9" s="3">
+      <c r="R11" s="3">
         <f t="shared" si="4"/>
         <v>4.9999999999999822E-2</v>
       </c>
-      <c r="Q9" s="3">
-        <v>127.57</v>
-      </c>
-      <c r="R9" s="3">
-        <v>-24.1</v>
-      </c>
-      <c r="S9" s="3">
+      <c r="S11" s="3">
+        <v>108.08</v>
+      </c>
+      <c r="T11" s="3">
+        <v>-7.76</v>
+      </c>
+      <c r="U11" s="3">
         <f t="shared" si="5"/>
-        <v>-3.4699999999999918</v>
-      </c>
-      <c r="T9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="U9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="V9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="W9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="X9" s="3">
+        <v>-0.31999999999999851</v>
+      </c>
+      <c r="V11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="W11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="X11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z11" s="3">
         <v>528</v>
       </c>
-      <c r="Y9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z9" s="18">
+      <c r="AA11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB11" s="21">
         <v>1.23</v>
       </c>
-      <c r="AA9" s="18">
+      <c r="AC11" s="21">
         <v>1.06</v>
       </c>
-      <c r="AB9" s="18">
+      <c r="AD11" s="21">
         <v>0.77</v>
       </c>
-      <c r="AC9" s="18">
+      <c r="AE11" s="21">
         <v>0.94</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B12" s="3">
         <v>2.1800000000000002</v>
       </c>
-      <c r="C10" s="3">
-        <v>2.42</v>
-      </c>
-      <c r="D10" s="7">
+      <c r="C12" s="3">
+        <v>2.41</v>
+      </c>
+      <c r="D12" s="7">
+        <f t="shared" si="0"/>
+        <v>9.5435684647302885E-2</v>
+      </c>
+      <c r="E12" s="3">
+        <v>2.79</v>
+      </c>
+      <c r="F12" s="3">
+        <v>1.84</v>
+      </c>
+      <c r="G12" s="7">
         <f t="shared" si="1"/>
-        <v>9.917355371900817E-2</v>
-      </c>
-      <c r="E10" s="3">
-        <v>3</v>
-      </c>
-      <c r="F10" s="3">
-        <v>1.63</v>
-      </c>
-      <c r="G10" s="7">
+        <v>-0.51630434782608692</v>
+      </c>
+      <c r="H12" s="3">
+        <v>3.52</v>
+      </c>
+      <c r="I12" s="3">
+        <v>7.43</v>
+      </c>
+      <c r="J12" s="31">
         <f t="shared" si="2"/>
-        <v>-0.84049079754601241</v>
-      </c>
-      <c r="H10" s="3">
-        <v>3.24</v>
-      </c>
-      <c r="I10" s="3">
-        <v>3.7</v>
-      </c>
-      <c r="J10" s="7">
-        <f t="shared" si="0"/>
-        <v>0.1243243243243243</v>
-      </c>
-      <c r="K10" s="3">
+        <v>0.47375504710632571</v>
+      </c>
+      <c r="K12" s="25">
+        <v>7.32</v>
+      </c>
+      <c r="L12" s="29">
+        <f>(I12-K12)/I12</f>
+        <v>1.4804845222072602E-2</v>
+      </c>
+      <c r="M12" s="3">
         <v>-1.62</v>
       </c>
-      <c r="L10" s="3">
+      <c r="N12" s="3">
         <v>-1.46</v>
       </c>
-      <c r="M10" s="7">
+      <c r="O12" s="7">
         <f t="shared" si="3"/>
         <v>-0.10958904109589052</v>
       </c>
-      <c r="N10" s="3">
+      <c r="P12" s="3">
         <v>2.64</v>
       </c>
-      <c r="O10" s="3">
+      <c r="Q12" s="3">
         <v>2.42</v>
       </c>
-      <c r="P10" s="3">
+      <c r="R12" s="3">
         <f t="shared" si="4"/>
         <v>0.2200000000000002</v>
       </c>
-      <c r="Q10" s="3">
-        <v>112.89</v>
-      </c>
-      <c r="R10" s="3">
-        <v>-11.07</v>
-      </c>
-      <c r="S10" s="3">
+      <c r="S12" s="3">
+        <v>113.96</v>
+      </c>
+      <c r="T12" s="3">
+        <v>-11.93</v>
+      </c>
+      <c r="U12" s="3">
         <f t="shared" si="5"/>
-        <v>-1.8200000000000003</v>
-      </c>
-      <c r="T10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="U10" s="3">
+        <v>-2.029999999999994</v>
+      </c>
+      <c r="V12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="W12" s="3">
         <v>-15.67</v>
       </c>
-      <c r="V10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="W10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="X10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z10" s="18">
+      <c r="X12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB12" s="21">
         <v>1.19</v>
       </c>
-      <c r="AA10" s="18">
+      <c r="AC12" s="21">
         <v>1.24</v>
       </c>
-      <c r="AB10" s="18">
+      <c r="AD12" s="21">
         <v>0.81</v>
       </c>
-      <c r="AC10" s="18">
+      <c r="AE12" s="21">
         <v>0.76</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B13" s="2">
         <v>2.48</v>
       </c>
-      <c r="C11" s="2">
-        <v>2.98</v>
-      </c>
-      <c r="D11" s="9">
+      <c r="C13" s="2">
+        <v>3.25</v>
+      </c>
+      <c r="D13" s="9">
+        <f t="shared" si="0"/>
+        <v>0.23692307692307693</v>
+      </c>
+      <c r="E13" s="2">
+        <v>-0.28000000000000003</v>
+      </c>
+      <c r="F13" s="2">
+        <v>5.62</v>
+      </c>
+      <c r="G13" s="9">
         <f t="shared" si="1"/>
-        <v>0.16778523489932887</v>
-      </c>
-      <c r="E11" s="2">
-        <v>-0.5</v>
-      </c>
-      <c r="F11" s="2">
-        <v>5.38</v>
-      </c>
-      <c r="G11" s="9">
+        <v>1.0498220640569396</v>
+      </c>
+      <c r="H13" s="2">
+        <v>3.48</v>
+      </c>
+      <c r="I13" s="2">
+        <v>6.7</v>
+      </c>
+      <c r="J13" s="32">
         <f t="shared" si="2"/>
-        <v>1.0929368029739777</v>
-      </c>
-      <c r="H11" s="2">
-        <v>3.42</v>
-      </c>
-      <c r="I11" s="2">
-        <v>3.58</v>
-      </c>
-      <c r="J11" s="9">
-        <f t="shared" si="0"/>
-        <v>4.4692737430167634E-2</v>
-      </c>
-      <c r="K11" s="2">
+        <v>0.5194029850746269</v>
+      </c>
+      <c r="K13" s="26">
+        <v>7.65</v>
+      </c>
+      <c r="L13" s="29">
+        <f>(I13-K13)/I13</f>
+        <v>-0.14179104477611942</v>
+      </c>
+      <c r="M13" s="2">
         <v>-1.4</v>
       </c>
-      <c r="L11" s="2">
+      <c r="N13" s="2">
         <v>-1.07</v>
       </c>
-      <c r="M11" s="9">
+      <c r="O13" s="9">
         <f t="shared" si="3"/>
         <v>-0.3084112149532709</v>
       </c>
-      <c r="N11" s="2">
+      <c r="P13" s="2">
         <v>3.71</v>
       </c>
-      <c r="O11" s="2">
+      <c r="Q13" s="2">
         <v>2.1800000000000002</v>
       </c>
-      <c r="P11" s="2">
+      <c r="R13" s="2">
         <f t="shared" si="4"/>
         <v>1.5299999999999998</v>
       </c>
-      <c r="Q11" s="2">
-        <v>34.76</v>
-      </c>
-      <c r="R11" s="2">
-        <v>82.56</v>
-      </c>
-      <c r="S11" s="2">
+      <c r="S13" s="2">
+        <v>49.5</v>
+      </c>
+      <c r="T13" s="2">
+        <v>69.739999999999995</v>
+      </c>
+      <c r="U13" s="2">
         <f t="shared" si="5"/>
-        <v>-17.319999999999993</v>
-      </c>
-      <c r="T11" s="2">
+        <v>-19.239999999999995</v>
+      </c>
+      <c r="V13" s="2">
         <v>-19.16</v>
       </c>
-      <c r="U11" s="2">
+      <c r="W13" s="2">
         <v>-20.27</v>
       </c>
-      <c r="V11" s="10">
+      <c r="X13" s="10">
         <f t="shared" si="6"/>
         <v>0.94523926985693141</v>
       </c>
-      <c r="W11" s="2">
+      <c r="Y13" s="2">
         <v>919</v>
       </c>
-      <c r="X11" s="2">
+      <c r="Z13" s="2">
         <v>796</v>
       </c>
-      <c r="Y11" s="2">
+      <c r="AA13" s="2">
         <f t="shared" si="7"/>
         <v>123</v>
       </c>
-      <c r="Z11" s="19">
+      <c r="AB13" s="22">
         <v>0.6</v>
       </c>
-      <c r="AA11" s="19">
+      <c r="AC13" s="22">
         <v>0.73</v>
       </c>
-      <c r="AB11" s="20">
+      <c r="AD13" s="23">
         <v>1.4</v>
       </c>
-      <c r="AC11" s="19">
+      <c r="AE13" s="22">
         <v>1.27</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="6">
-        <f>AVERAGE(B4,B6:B10)</f>
-        <v>3.4350000000000001</v>
-      </c>
-      <c r="C12" s="6">
-        <f t="shared" ref="C12:S12" si="8">AVERAGE(C4,C6:C10)</f>
-        <v>3.7216666666666662</v>
-      </c>
-      <c r="D12" s="6">
-        <f>AVERAGE(D4,D6:D10)*100</f>
-        <v>6.507064594838015</v>
-      </c>
-      <c r="E12" s="6">
+      <c r="B14" s="6">
+        <f>AVERAGE(B4,B6:B12)</f>
+        <v>3.4974999999999996</v>
+      </c>
+      <c r="C14" s="6">
+        <f>AVERAGE(C4,C6:C12)</f>
+        <v>3.82</v>
+      </c>
+      <c r="D14" s="6">
+        <f>AVERAGE(D4,D6:D12)*100</f>
+        <v>6.9925227290997043</v>
+      </c>
+      <c r="E14" s="6">
+        <f>AVERAGE(E4,E6:E12)</f>
+        <v>5.36625</v>
+      </c>
+      <c r="F14" s="6">
+        <f>AVERAGE(F4,F6:F12)</f>
+        <v>4.6612499999999999</v>
+      </c>
+      <c r="G14" s="6">
+        <f>AVERAGE(G4,G6, G7, G9:G12)*100</f>
+        <v>-20.782268605693353</v>
+      </c>
+      <c r="H14" s="6">
+        <f>AVERAGE(H4,H6:H12)</f>
+        <v>3.5787499999999999</v>
+      </c>
+      <c r="I14" s="6">
+        <f>AVERAGE(I4,I6:I12)</f>
+        <v>7.3287500000000003</v>
+      </c>
+      <c r="J14" s="12">
+        <f>AVERAGE(J4,J6:J12)</f>
+        <v>0.48843955468674044</v>
+      </c>
+      <c r="K14" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="L14" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="M14" s="6">
+        <f>AVERAGE(M4,M6:M12)</f>
+        <v>-1.1212499999999999</v>
+      </c>
+      <c r="N14" s="6">
+        <f>AVERAGE(N4,N6:N12)</f>
+        <v>-1.0550000000000002</v>
+      </c>
+      <c r="O14" s="6">
+        <f>AVERAGE(O4,O6:O12)*100</f>
+        <v>-8.2010701509663004</v>
+      </c>
+      <c r="P14" s="6">
+        <f t="shared" ref="P14:U14" si="8">AVERAGE(P4,P6:P12)</f>
+        <v>1.8537499999999998</v>
+      </c>
+      <c r="Q14" s="6">
         <f t="shared" si="8"/>
-        <v>5.04</v>
-      </c>
-      <c r="F12" s="6">
+        <v>1.9037500000000001</v>
+      </c>
+      <c r="R14" s="12">
         <f t="shared" si="8"/>
-        <v>4.2350000000000003</v>
-      </c>
-      <c r="G12" s="6">
-        <f>AVERAGE(G4,G6:G10)*100</f>
-        <v>-32.788654942396221</v>
-      </c>
-      <c r="H12" s="6">
-        <f t="shared" si="8"/>
-        <v>3.8266666666666667</v>
-      </c>
-      <c r="I12" s="6">
-        <f t="shared" si="8"/>
-        <v>3.6833333333333331</v>
-      </c>
-      <c r="J12" s="6">
-        <f>AVERAGE(J4,J6:J10)*100</f>
-        <v>-3.8943794167800339</v>
-      </c>
-      <c r="K12" s="6">
-        <f t="shared" si="8"/>
-        <v>-1.1316666666666666</v>
-      </c>
-      <c r="L12" s="6">
-        <f t="shared" si="8"/>
-        <v>-1.0383333333333333</v>
-      </c>
-      <c r="M12" s="6">
-        <f>AVERAGE(M4,M6:M10)*100</f>
-        <v>-10.265253201897041</v>
-      </c>
-      <c r="N12" s="6">
-        <f t="shared" si="8"/>
-        <v>1.9433333333333334</v>
-      </c>
-      <c r="O12" s="6">
-        <f t="shared" si="8"/>
-        <v>1.9266666666666667</v>
-      </c>
-      <c r="P12" s="12">
-        <f t="shared" si="8"/>
-        <v>1.6666666666666607E-2</v>
-      </c>
-      <c r="Q12" s="6">
-        <f t="shared" si="8"/>
-        <v>108.77666666666666</v>
-      </c>
-      <c r="R12" s="6">
-        <f t="shared" si="8"/>
-        <v>-9.3883333333333319</v>
-      </c>
-      <c r="S12" s="6">
-        <f t="shared" si="8"/>
-        <v>0.61166666666666691</v>
-      </c>
-      <c r="T12" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="U12" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="V12" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="W12" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="X12" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y12" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z12" s="6">
-        <f t="shared" ref="Z12:AA12" si="9">AVERAGE(Z4,Z6:Z10)</f>
+        <v>-5.0000000000000072E-2</v>
+      </c>
+      <c r="S14" s="6">
+        <f>AVERAGE(S4,S6:S12)</f>
+        <v>102.84875000000001</v>
+      </c>
+      <c r="T14" s="6">
+        <f>AVERAGE(T4,T6:T12)</f>
+        <v>-3.1087500000000006</v>
+      </c>
+      <c r="U14" s="6">
+        <f>AVERAGE(U4,U6:U12)</f>
+        <v>0.26000000000000267</v>
+      </c>
+      <c r="V14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="W14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="X14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB14" s="6">
+        <f t="shared" ref="AB14:AC14" si="9">AVERAGE(AB4,AB6:AB12)</f>
         <v>1.1199999999999999</v>
       </c>
-      <c r="AA12" s="6">
+      <c r="AC14" s="6">
         <f t="shared" si="9"/>
         <v>0.97166666666666668</v>
       </c>
-      <c r="AB12" s="6">
-        <f t="shared" ref="AB12:AC12" si="10">AVERAGE(AB4,AB6:AB10)</f>
+      <c r="AD14" s="6">
+        <f t="shared" ref="AD14:AE14" si="10">AVERAGE(AD4,AD6:AD12)</f>
         <v>0.88000000000000023</v>
       </c>
-      <c r="AC12" s="6">
+      <c r="AE14" s="6">
         <f t="shared" si="10"/>
         <v>1.0283333333333333</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="1">
-        <f>STDEV(B4,B6:B10)</f>
-        <v>0.98441353099192985</v>
-      </c>
-      <c r="C13" s="1">
-        <f t="shared" ref="C13:S13" si="11">STDEV(C4,C6:C10)</f>
-        <v>1.2365179605111556</v>
-      </c>
-      <c r="D13" s="1">
-        <f>STDEV(D4,D6:D10)*100</f>
-        <v>6.2982923144502516</v>
-      </c>
-      <c r="E13" s="1">
+      <c r="B15" s="1">
+        <f>STDEV(B4,B6:B12)</f>
+        <v>1.055269092290142</v>
+      </c>
+      <c r="C15" s="1">
+        <f>STDEV(C4,C6:C12)</f>
+        <v>1.3107576870977018</v>
+      </c>
+      <c r="D15" s="1">
+        <f>STDEV(D4,D6:D12)*100</f>
+        <v>7.1851918136864246</v>
+      </c>
+      <c r="E15" s="1">
+        <f>STDEV(E4,E6:E12)</f>
+        <v>2.2678809335085099</v>
+      </c>
+      <c r="F15" s="1">
+        <f>STDEV(F4,F6:F12)</f>
+        <v>2.9386120995171474</v>
+      </c>
+      <c r="G15" s="1">
+        <f>STDEV(G4,G6, G7, G9:G12)*100</f>
+        <v>37.045559614634122</v>
+      </c>
+      <c r="H15" s="1">
+        <f>STDEV(H4,H6:H12)</f>
+        <v>0.19635518109501757</v>
+      </c>
+      <c r="I15" s="1">
+        <f>STDEV(I4,I6:I12)</f>
+        <v>0.30291146749975828</v>
+      </c>
+      <c r="J15" s="18">
+        <f>STDEV(J4,J6:J12)</f>
+        <v>2.161808244836597E-2</v>
+      </c>
+      <c r="K15" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="L15" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="M15" s="1">
+        <f>STDEV(M4,M6:M12)</f>
+        <v>0.37566845184854974</v>
+      </c>
+      <c r="N15" s="1">
+        <f>STDEV(N4,N6:N12)</f>
+        <v>0.40422765862815419</v>
+      </c>
+      <c r="O15" s="1">
+        <f>STDEV(O4,O6:O12)*100</f>
+        <v>8.3625067687289523</v>
+      </c>
+      <c r="P15" s="1">
+        <f t="shared" ref="P15:U15" si="11">STDEV(P4,P6:P12)</f>
+        <v>0.43220158986948998</v>
+      </c>
+      <c r="Q15" s="1">
         <f t="shared" si="11"/>
-        <v>1.7410801245204084</v>
-      </c>
-      <c r="F13" s="1">
+        <v>0.41665119018876529</v>
+      </c>
+      <c r="R15" s="1">
         <f t="shared" si="11"/>
-        <v>2.0381732016685925</v>
-      </c>
-      <c r="G13" s="1">
-        <f>STDEV(G4,G6:G10)*100</f>
-        <v>43.812154462427948</v>
-      </c>
-      <c r="H13" s="1">
+        <v>0.28390139133156789</v>
+      </c>
+      <c r="S15" s="1">
         <f t="shared" si="11"/>
-        <v>0.3245715124077691</v>
-      </c>
-      <c r="I13" s="1">
+        <v>87.261207947747323</v>
+      </c>
+      <c r="T15" s="1">
         <f t="shared" si="11"/>
-        <v>7.5011110288187674E-2</v>
-      </c>
-      <c r="J13" s="1">
-        <f>STDEV(J4,J6:J10)*100</f>
-        <v>8.5484823010712105</v>
-      </c>
-      <c r="K13" s="1">
+        <v>87.423137087468362</v>
+      </c>
+      <c r="U15" s="1">
         <f t="shared" si="11"/>
-        <v>0.36030080025815492</v>
-      </c>
-      <c r="L13" s="1">
-        <f t="shared" si="11"/>
-        <v>0.36515293599623</v>
-      </c>
-      <c r="M13" s="1">
-        <f>STDEV(M4,M6:M10)*100</f>
-        <v>7.3435167619276456</v>
-      </c>
-      <c r="N13" s="1">
-        <f t="shared" si="11"/>
-        <v>0.46193794677063094</v>
-      </c>
-      <c r="O13" s="1">
-        <f t="shared" si="11"/>
-        <v>0.46089767483321836</v>
-      </c>
-      <c r="P13" s="1">
-        <f t="shared" si="11"/>
-        <v>0.14472963299430674</v>
-      </c>
-      <c r="Q13" s="1">
-        <f t="shared" si="11"/>
-        <v>39.853173859388797</v>
-      </c>
-      <c r="R13" s="1">
-        <f t="shared" si="11"/>
-        <v>39.715295500180616</v>
-      </c>
-      <c r="S13" s="1">
-        <f t="shared" si="11"/>
-        <v>2.7200545337670432</v>
-      </c>
-      <c r="T13" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="U13" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="V13" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="W13" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="X13" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y13" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z13" s="1">
-        <f>STDEV(Z4,Z6:Z10)</f>
+        <v>3.2626457274514418</v>
+      </c>
+      <c r="V15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="W15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="X15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB15" s="1">
+        <f>STDEV(AB4,AB6:AB12)</f>
         <v>0.14560219778561151</v>
       </c>
-      <c r="AA13" s="1">
-        <f>STDEV(AA4,AA6:AA10)</f>
+      <c r="AC15" s="1">
+        <f>STDEV(AC4,AC6:AC12)</f>
         <v>0.18956968815363603</v>
       </c>
-      <c r="AB13" s="1">
-        <f>STDEV(AB4,AB6:AB10)</f>
+      <c r="AD15" s="1">
+        <f>STDEV(AD4,AD6:AD12)</f>
         <v>0.14560219778560907</v>
       </c>
-      <c r="AC13" s="1">
-        <f>STDEV(AC4,AC6:AC10)</f>
+      <c r="AE15" s="1">
+        <f>STDEV(AE4,AE6:AE12)</f>
         <v>0.18956968815363556</v>
       </c>
+    </row>
+    <row r="17" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A17"/>
+    </row>
+    <row r="19" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A19" s="20"/>
+    </row>
+    <row r="20" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A20"/>
+    </row>
+    <row r="21" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A21"/>
+    </row>
+    <row r="22" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A22"/>
+    </row>
+    <row r="23" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A23"/>
+    </row>
+    <row r="24" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A24"/>
+    </row>
+    <row r="25" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A25"/>
+    </row>
+    <row r="26" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A26"/>
+    </row>
+    <row r="27" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A27"/>
+    </row>
+    <row r="28" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A28"/>
+    </row>
+    <row r="29" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A29"/>
+    </row>
+    <row r="30" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A30"/>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="Z1:AA1"/>
     <mergeCell ref="AB1:AC1"/>
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="T1:V1"/>
-    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="AD1:AE1"/>
+    <mergeCell ref="H1:L1"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="P1:R1"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="S1:U1"/>
+    <mergeCell ref="V1:X1"/>
+    <mergeCell ref="Y1:AA1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>